<commit_message>
Datos en formato .csv
</commit_message>
<xml_diff>
--- a/Datos/Var_Crecimiento.xlsx
+++ b/Datos/Var_Crecimiento.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29328"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29426"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://estunaedu-my.sharepoint.com/personal/victor_rsalguera_ci_una_edu_ni/Documents/Artículos científicos/Promotores de crecimiento/Base de datos/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Analisis_inoculantes\Iniculantes\Datos\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="159" documentId="8_{55D3953B-F51B-47D3-8FF1-A6C83C5DB6E8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{DA45049B-6B4A-4C79-8297-103149C55068}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F53BD746-ACD4-448C-B67B-DB32BF7DBF5E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{4EE320E4-0C14-4B08-92B2-957F09EB4025}"/>
   </bookViews>
@@ -108,10 +108,10 @@
     <t>Altura</t>
   </si>
   <si>
-    <t>Numero de hojas</t>
+    <t>Diametro</t>
   </si>
   <si>
-    <t>Diametro</t>
+    <t>Numero_de_hojas</t>
   </si>
 </sst>
 </file>
@@ -189,23 +189,7 @@
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="5">
-    <dxf>
-      <numFmt numFmtId="171" formatCode="0.0"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="171" formatCode="0.0"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="171" formatCode="0.0"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="171" formatCode="0.0"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="2" formatCode="0.00"/>
-    </dxf>
-  </dxfs>
+  <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
@@ -538,7 +522,7 @@
   <dimension ref="A1:E33"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D1" sqref="D1"/>
+      <selection activeCell="K16" sqref="K16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -558,10 +542,10 @@
         <v>22</v>
       </c>
       <c r="D1" s="7" t="s">
+        <v>24</v>
+      </c>
+      <c r="E1" s="7" t="s">
         <v>23</v>
-      </c>
-      <c r="E1" s="7" t="s">
-        <v>24</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
@@ -11145,6 +11129,68 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <AppVersion xmlns="76c649a7-3579-457d-82e1-ba18b3f1caa8" xsi:nil="true"/>
+    <TeamsChannelId xmlns="76c649a7-3579-457d-82e1-ba18b3f1caa8" xsi:nil="true"/>
+    <Invited_Students xmlns="76c649a7-3579-457d-82e1-ba18b3f1caa8" xsi:nil="true"/>
+    <IsNotebookLocked xmlns="76c649a7-3579-457d-82e1-ba18b3f1caa8" xsi:nil="true"/>
+    <DefaultSectionNames xmlns="76c649a7-3579-457d-82e1-ba18b3f1caa8" xsi:nil="true"/>
+    <FolderType xmlns="76c649a7-3579-457d-82e1-ba18b3f1caa8" xsi:nil="true"/>
+    <CultureName xmlns="76c649a7-3579-457d-82e1-ba18b3f1caa8" xsi:nil="true"/>
+    <LMS_Mappings xmlns="76c649a7-3579-457d-82e1-ba18b3f1caa8" xsi:nil="true"/>
+    <Is_Collaboration_Space_Locked xmlns="76c649a7-3579-457d-82e1-ba18b3f1caa8" xsi:nil="true"/>
+    <Teams_Channel_Section_Location xmlns="76c649a7-3579-457d-82e1-ba18b3f1caa8" xsi:nil="true"/>
+    <Math_Settings xmlns="76c649a7-3579-457d-82e1-ba18b3f1caa8" xsi:nil="true"/>
+    <Templates xmlns="76c649a7-3579-457d-82e1-ba18b3f1caa8" xsi:nil="true"/>
+    <Self_Registration_Enabled xmlns="76c649a7-3579-457d-82e1-ba18b3f1caa8" xsi:nil="true"/>
+    <Teachers xmlns="76c649a7-3579-457d-82e1-ba18b3f1caa8">
+      <UserInfo>
+        <DisplayName/>
+        <AccountId xsi:nil="true"/>
+        <AccountType/>
+      </UserInfo>
+    </Teachers>
+    <Students xmlns="76c649a7-3579-457d-82e1-ba18b3f1caa8">
+      <UserInfo>
+        <DisplayName/>
+        <AccountId xsi:nil="true"/>
+        <AccountType/>
+      </UserInfo>
+    </Students>
+    <Student_Groups xmlns="76c649a7-3579-457d-82e1-ba18b3f1caa8">
+      <UserInfo>
+        <DisplayName/>
+        <AccountId xsi:nil="true"/>
+        <AccountType/>
+      </UserInfo>
+    </Student_Groups>
+    <Invited_Teachers xmlns="76c649a7-3579-457d-82e1-ba18b3f1caa8" xsi:nil="true"/>
+    <Has_Teacher_Only_SectionGroup xmlns="76c649a7-3579-457d-82e1-ba18b3f1caa8" xsi:nil="true"/>
+    <NotebookType xmlns="76c649a7-3579-457d-82e1-ba18b3f1caa8" xsi:nil="true"/>
+    <_activity xmlns="76c649a7-3579-457d-82e1-ba18b3f1caa8" xsi:nil="true"/>
+    <Owner xmlns="76c649a7-3579-457d-82e1-ba18b3f1caa8">
+      <UserInfo>
+        <DisplayName/>
+        <AccountId xsi:nil="true"/>
+        <AccountType/>
+      </UserInfo>
+    </Owner>
+    <Distribution_Groups xmlns="76c649a7-3579-457d-82e1-ba18b3f1caa8" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x01010056AFEAF56BF629418C73F8DDEE3FF0A5" ma:contentTypeVersion="40" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="095dd3fe2d6a3eab44093e57d57799d6">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns3="76c649a7-3579-457d-82e1-ba18b3f1caa8" xmlns:ns4="7cbcdc4f-0d47-4092-9780-53f7000a4db0" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="5ee522b0ebb16cf80cc7eb7982cfd126" ns3:_="" ns4:_="">
     <xsd:import namespace="76c649a7-3579-457d-82e1-ba18b3f1caa8"/>
@@ -11597,69 +11643,32 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{DFC0F7B7-7AEB-4B71-BEAD-9EC67B92AB2A}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="76c649a7-3579-457d-82e1-ba18b3f1caa8"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="7cbcdc4f-0d47-4092-9780-53f7000a4db0"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <AppVersion xmlns="76c649a7-3579-457d-82e1-ba18b3f1caa8" xsi:nil="true"/>
-    <TeamsChannelId xmlns="76c649a7-3579-457d-82e1-ba18b3f1caa8" xsi:nil="true"/>
-    <Invited_Students xmlns="76c649a7-3579-457d-82e1-ba18b3f1caa8" xsi:nil="true"/>
-    <IsNotebookLocked xmlns="76c649a7-3579-457d-82e1-ba18b3f1caa8" xsi:nil="true"/>
-    <DefaultSectionNames xmlns="76c649a7-3579-457d-82e1-ba18b3f1caa8" xsi:nil="true"/>
-    <FolderType xmlns="76c649a7-3579-457d-82e1-ba18b3f1caa8" xsi:nil="true"/>
-    <CultureName xmlns="76c649a7-3579-457d-82e1-ba18b3f1caa8" xsi:nil="true"/>
-    <LMS_Mappings xmlns="76c649a7-3579-457d-82e1-ba18b3f1caa8" xsi:nil="true"/>
-    <Is_Collaboration_Space_Locked xmlns="76c649a7-3579-457d-82e1-ba18b3f1caa8" xsi:nil="true"/>
-    <Teams_Channel_Section_Location xmlns="76c649a7-3579-457d-82e1-ba18b3f1caa8" xsi:nil="true"/>
-    <Math_Settings xmlns="76c649a7-3579-457d-82e1-ba18b3f1caa8" xsi:nil="true"/>
-    <Templates xmlns="76c649a7-3579-457d-82e1-ba18b3f1caa8" xsi:nil="true"/>
-    <Self_Registration_Enabled xmlns="76c649a7-3579-457d-82e1-ba18b3f1caa8" xsi:nil="true"/>
-    <Teachers xmlns="76c649a7-3579-457d-82e1-ba18b3f1caa8">
-      <UserInfo>
-        <DisplayName/>
-        <AccountId xsi:nil="true"/>
-        <AccountType/>
-      </UserInfo>
-    </Teachers>
-    <Students xmlns="76c649a7-3579-457d-82e1-ba18b3f1caa8">
-      <UserInfo>
-        <DisplayName/>
-        <AccountId xsi:nil="true"/>
-        <AccountType/>
-      </UserInfo>
-    </Students>
-    <Student_Groups xmlns="76c649a7-3579-457d-82e1-ba18b3f1caa8">
-      <UserInfo>
-        <DisplayName/>
-        <AccountId xsi:nil="true"/>
-        <AccountType/>
-      </UserInfo>
-    </Student_Groups>
-    <Invited_Teachers xmlns="76c649a7-3579-457d-82e1-ba18b3f1caa8" xsi:nil="true"/>
-    <Has_Teacher_Only_SectionGroup xmlns="76c649a7-3579-457d-82e1-ba18b3f1caa8" xsi:nil="true"/>
-    <NotebookType xmlns="76c649a7-3579-457d-82e1-ba18b3f1caa8" xsi:nil="true"/>
-    <_activity xmlns="76c649a7-3579-457d-82e1-ba18b3f1caa8" xsi:nil="true"/>
-    <Owner xmlns="76c649a7-3579-457d-82e1-ba18b3f1caa8">
-      <UserInfo>
-        <DisplayName/>
-        <AccountId xsi:nil="true"/>
-        <AccountType/>
-      </UserInfo>
-    </Owner>
-    <Distribution_Groups xmlns="76c649a7-3579-457d-82e1-ba18b3f1caa8" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{2E70056D-9C57-406E-8566-DE6276DB3A60}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{4E42788C-65B8-4480-88DB-DE3F2DB5630D}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -11676,29 +11685,4 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{2E70056D-9C57-406E-8566-DE6276DB3A60}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{DFC0F7B7-7AEB-4B71-BEAD-9EC67B92AB2A}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="76c649a7-3579-457d-82e1-ba18b3f1caa8"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="7cbcdc4f-0d47-4092-9780-53f7000a4db0"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
 </file>
</xml_diff>